<commit_message>
updated word2vec code 2
</commit_message>
<xml_diff>
--- a/NLP_Transfer_Learning_Methods/Word2Vec/Frequent_Words_and_Clusters.xlsx
+++ b/NLP_Transfer_Learning_Methods/Word2Vec/Frequent_Words_and_Clusters.xlsx
@@ -1709,7 +1709,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>income, corporation, interest, stock, foreign, business, return, gross, except, election</t>
+          <t>property, corporation, interest, stock, foreign, business, item, basis, without, loss</t>
         </is>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>shall, respect, property, term, person, qualified, described, states, united, taxpayer</t>
+          <t>purposes, term, case, general, qualified, described, apply, means, provided, defined</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>tax, purposes, case, general, treated, stat, apply, means, provided, defined</t>
+          <t>shall, subsection, paragraph, person, subparagraph, stat, states, united, percent, trust</t>
         </is>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>year, taxable, subsection, amount, paragraph, plan, subparagraph, period, date, made</t>
+          <t>year, taxable, amount, tax, respect, income, plan, treated, period, date</t>
         </is>
       </c>
     </row>
@@ -1762,7 +1762,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>secretary, regulations</t>
+          <t>secretary, may, regulations, return, required, information</t>
         </is>
       </c>
     </row>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>shall, subsection, amount, paragraph, income, property, corporation, plan, person, may</t>
+          <t>shall, subsection, amount, paragraph, respect, income, property, corporation, plan, person</t>
         </is>
       </c>
     </row>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>purposes, respect, term, case, general, described, qualified, treated, states, apply</t>
+          <t>purposes, term, case, general, described, qualified, treated, apply, made, means</t>
         </is>
       </c>
     </row>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>tax, stat, foreign, credit, certain, item, part, deduction, act, special</t>
+          <t>tax, stat, states, foreign, credit, certain, item, part, deduction, act</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>year, taxable, date, period, years, calendar, service, beginning, day</t>
+          <t>year, taxable, date, period, percent, business, years, loss, calendar, beginning</t>
         </is>
       </c>
     </row>

</xml_diff>